<commit_message>
COmpleted code that returns results to the data excel when it runs at set times of the data Last step is to implement thecode to calculates its own implied volatility so that I dont get errors when I run the code for the current day options.
</commit_message>
<xml_diff>
--- a/hpReturnData.xlsx
+++ b/hpReturnData.xlsx
@@ -1,39 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Trading Date</t>
+  </si>
+  <si>
+    <t>Gamma Imblanace</t>
+  </si>
+  <si>
+    <t>Hedge Pressure</t>
+  </si>
+  <si>
+    <t>12:30 to close return</t>
+  </si>
+  <si>
+    <t>t+1 first 30 return</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,92 +76,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -429,136 +393,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="12.29071428571429" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="14.86214285714286" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-    <col width="17.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="16.71928571428571" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col min="1" max="1" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Trading Date</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Gamma Imblanace</t>
-        </is>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Hedge Pressure</t>
-        </is>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>12:30 to close return</t>
-        </is>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>t+1 first 30 return</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing excel data sheet
</commit_message>
<xml_diff>
--- a/hpReturnData.xlsx
+++ b/hpReturnData.xlsx
@@ -1,45 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Trading Date</t>
+  </si>
+  <si>
+    <t>Gamma Imblanace</t>
+  </si>
+  <si>
+    <t>Hedge Pressure</t>
+  </si>
+  <si>
+    <t>t-1 to 12:30 return</t>
+  </si>
+  <si>
+    <t>12:30 to close return</t>
+  </si>
+  <si>
+    <t>t+1 first 30 return</t>
+  </si>
+  <si>
+    <t>06/29/23</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>0.10282%</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,98 +94,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,70 +414,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="12.29071428571429" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="14.86214285714286" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="17.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="16.71928571428571" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
+    <col min="1" max="1" style="5" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Trading Date</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Gamma Imblanace</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Hedge Pressure</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>12:30 to close return</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>t+1 first 30 return</t>
-        </is>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4">
         <v>0.0256</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4">
         <v>0.00763</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.10282%</t>
-        </is>
-      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Editing Return Calculations to fit research paper
</commit_message>
<xml_diff>
--- a/hpReturnData.xlsx
+++ b/hpReturnData.xlsx
@@ -1,45 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Mercy\vscode\SmartMoneyAlgo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2F917-A60A-4F43-B97C-33F6B8AA1E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Trading Date</t>
+  </si>
+  <si>
+    <t>Gamma Imblanace</t>
+  </si>
+  <si>
+    <t>Hedge Pressure</t>
+  </si>
+  <si>
+    <t>t-1 to 12:30 return %</t>
+  </si>
+  <si>
+    <t>12:30 to close return %</t>
+  </si>
+  <si>
+    <t>t+1 first 30 return %</t>
+  </si>
+  <si>
+    <t>06/29/23</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>0.10282%</t>
+  </si>
+  <si>
+    <t>07/03/23</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,93 +105,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -439,102 +420,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="12.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="14.85546875" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="19" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="21.140625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="16.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Trading Date</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Gamma Imblanace</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Hedge Pressure</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>t-1 to 12:30 return %</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>12:30 to close return %</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>t+1 first 30 return %</t>
-        </is>
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>06/29/23</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>0.0256</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>0.00763</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>na</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.10282%</t>
-        </is>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>7.6299999999999996E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>07/03/23</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.00192</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.00022</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.001150536381134866</v>
-      </c>
-      <c r="E3" s="5" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>-1.92E-3</v>
+      </c>
+      <c r="C3">
+        <v>-2.2000000000000001E-4</v>
+      </c>
+      <c r="D3">
+        <v>1.150536381134866E-3</v>
+      </c>
+      <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.19642</v>
+      <c r="F3">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating code to run on this computer
</commit_message>
<xml_diff>
--- a/hpReturnData.xlsx
+++ b/hpReturnData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Mercy\vscode\SmartMoneyAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2F917-A60A-4F43-B97C-33F6B8AA1E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E28997-40CB-437C-8EC8-BA60CE134319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -119,6 +119,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +425,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +498,13 @@
         <v>-0.4</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>